<commit_message>
5 verstopte waardes nu ook aangepast.
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.91 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.91 waardelijsten.xlsx
@@ -3622,13 +3622,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34:G38"/>
+      <selection pane="bottomLeft" activeCell="I326" sqref="I326:I334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5616,7 +5615,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1">
+    <row r="67" spans="1:9">
       <c r="A67" s="1"/>
       <c r="B67" s="18" t="s">
         <v>703</v>
@@ -5641,7 +5640,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/EffectScenarionType/brandbaar</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9">
       <c r="A68" s="1"/>
       <c r="B68" s="18" t="s">
         <v>703</v>
@@ -5666,7 +5665,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/EffectScenarionType/explosief</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9">
       <c r="A69" s="1"/>
       <c r="B69" s="18" t="s">
         <v>703</v>
@@ -5691,7 +5690,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/EffectScenarionType/toxisch</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1">
+    <row r="70" spans="1:9">
       <c r="A70" s="1"/>
       <c r="B70" s="18" t="s">
         <v>703</v>
@@ -5923,7 +5922,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/EigenTopografieStatusValue/bestaand</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="28">
+    <row r="78" spans="1:9" ht="29" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>338</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/EigenTopografieStatusValue/plan</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="79" spans="1:9" ht="15" thickBot="1">
       <c r="A79" t="s">
         <v>496</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/aarding</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="80" spans="1:9" ht="15" thickBot="1">
       <c r="A80" t="s">
         <v>496</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/mof</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="81" spans="1:9" ht="15" thickBot="1">
       <c r="A81" t="s">
         <v>496</v>
       </c>
@@ -6043,7 +6042,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/hoogteligging</v>
       </c>
     </row>
-    <row r="82" spans="1:9" s="39" customFormat="1" ht="15" hidden="1" thickBot="1">
+    <row r="82" spans="1:9" s="39" customFormat="1" ht="15" thickBot="1">
       <c r="A82" t="s">
         <v>496</v>
       </c>
@@ -6073,7 +6072,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/adrespunt</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="83" spans="1:9" s="39" customFormat="1">
       <c r="A83" t="s">
         <v>496</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/connectionBox</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="84" spans="1:9" s="39" customFormat="1">
       <c r="A84" t="s">
         <v>496</v>
       </c>
@@ -6133,7 +6132,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="85" spans="1:9" s="39" customFormat="1">
       <c r="A85" t="s">
         <v>496</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/generator</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="86" spans="1:9" s="39" customFormat="1">
       <c r="A86" t="s">
         <v>496</v>
       </c>
@@ -6193,7 +6192,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/mainStation</v>
       </c>
     </row>
-    <row r="87" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="87" spans="1:9" s="39" customFormat="1">
       <c r="A87" t="s">
         <v>496</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/netStation</v>
       </c>
     </row>
-    <row r="88" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="88" spans="1:9" s="39" customFormat="1">
       <c r="A88" t="s">
         <v>496</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/streetLight</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="89" spans="1:9" s="39" customFormat="1">
       <c r="A89" t="s">
         <v>496</v>
       </c>
@@ -6283,7 +6282,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/subStation</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="90" spans="1:9" ht="15" thickBot="1">
       <c r="A90" t="s">
         <v>496</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/geulmof</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="28" hidden="1">
+    <row r="91" spans="1:9" ht="28">
       <c r="A91" t="s">
         <v>496</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>496</v>
       </c>
@@ -6373,7 +6372,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/kbInstallatie</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>496</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/kbEindpunt</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>496</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/kbContact</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="95" spans="1:9" ht="15" thickBot="1">
       <c r="A95" t="s">
         <v>496</v>
       </c>
@@ -6463,7 +6462,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ElectricityAppurtenanceTypeIMKLValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>339</v>
       </c>
@@ -6493,7 +6492,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/antenna</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>339</v>
       </c>
@@ -6523,7 +6522,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/termination</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>339</v>
       </c>
@@ -6553,7 +6552,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/handhole</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>339</v>
       </c>
@@ -6583,7 +6582,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/mof</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="100" spans="1:9" s="39" customFormat="1">
       <c r="A100" s="39" t="s">
         <v>339</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/nietBenoemd</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>339</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/kabelverdeler</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>339</v>
       </c>
@@ -6673,7 +6672,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/Stijgleiding</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="103" spans="1:9" s="39" customFormat="1">
       <c r="A103" s="39" t="s">
         <v>339</v>
       </c>
@@ -6703,7 +6702,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/GTWP</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>339</v>
       </c>
@@ -6733,7 +6732,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/afdekplaten</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>339</v>
       </c>
@@ -6763,7 +6762,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/doorvoerramen</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="106" spans="1:9" ht="15" thickBot="1">
       <c r="A106" t="s">
         <v>339</v>
       </c>
@@ -6790,7 +6789,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1">
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>339</v>
       </c>
@@ -6820,7 +6819,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsCableMaterialTypeValue/coaxial</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>339</v>
       </c>
@@ -6850,7 +6849,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsCableMaterialTypeValue/opticalFiber</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1">
+    <row r="109" spans="1:9" ht="15" thickBot="1">
       <c r="A109" t="s">
         <v>339</v>
       </c>
@@ -6880,7 +6879,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TelecommunicationsCableMaterialTypeValue/twistedPair</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="110" spans="1:9" ht="15" thickBot="1">
       <c r="A110" t="s">
         <v>442</v>
       </c>
@@ -6910,7 +6909,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/buis</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="111" spans="1:9" ht="15" thickBot="1">
       <c r="A111" t="s">
         <v>442</v>
       </c>
@@ -6940,7 +6939,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/bocht</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="112" spans="1:9" ht="15" thickBot="1">
       <c r="A112" t="s">
         <v>442</v>
       </c>
@@ -6970,7 +6969,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/tstuk</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="113" spans="1:9" ht="15" thickBot="1">
       <c r="A113" t="s">
         <v>442</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/bodem</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="114" spans="1:9" ht="15" thickBot="1">
       <c r="A114" t="s">
         <v>442</v>
       </c>
@@ -7030,7 +7029,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/lasnok</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="115" spans="1:9" ht="15" thickBot="1">
       <c r="A115" t="s">
         <v>442</v>
       </c>
@@ -7060,7 +7059,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/expansiestuk</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="116" spans="1:9" ht="15" thickBot="1">
       <c r="A116" t="s">
         <v>442</v>
       </c>
@@ -7090,7 +7089,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatieKoppeling</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="117" spans="1:9" ht="15" thickBot="1">
       <c r="A117" t="s">
         <v>442</v>
       </c>
@@ -7120,7 +7119,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/vloeistofvanger</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="118" spans="1:9" ht="15" thickBot="1">
       <c r="A118" t="s">
         <v>442</v>
       </c>
@@ -7150,7 +7149,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/raaginrichting</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="119" spans="1:9" ht="15" thickBot="1">
       <c r="A119" t="s">
         <v>442</v>
       </c>
@@ -7180,7 +7179,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/algemeenGasTransportOnderdeel</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="120" spans="1:9" ht="15" thickBot="1">
       <c r="A120" t="s">
         <v>442</v>
       </c>
@@ -7210,7 +7209,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductIMKLTypeValue/mud</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="121" spans="1:9" ht="15" thickBot="1">
       <c r="A121" t="s">
         <v>442</v>
       </c>
@@ -7240,7 +7239,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductIMKLTypeValue/methanol</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1">
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>442</v>
       </c>
@@ -7270,7 +7269,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductIMKLTypeValue/emulsie</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1">
+    <row r="123" spans="1:9" ht="15" thickBot="1">
       <c r="A123" t="s">
         <v>442</v>
       </c>
@@ -7300,7 +7299,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductIMKLTypeValue/glycol</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="124" spans="1:9" ht="15" thickBot="1">
       <c r="A124" t="s">
         <v>442</v>
       </c>
@@ -7330,7 +7329,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="125" spans="1:9" ht="15" thickBot="1">
       <c r="A125" t="s">
         <v>442</v>
       </c>
@@ -7360,7 +7359,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/ontluchting</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1">
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>442</v>
       </c>
@@ -7390,7 +7389,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/aftakzadel</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1">
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>442</v>
       </c>
@@ -7420,7 +7419,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/overgangsstuk</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1">
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>442</v>
       </c>
@@ -7450,7 +7449,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatiestuk</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1">
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>442</v>
       </c>
@@ -7480,7 +7479,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/ontspanningselement</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1">
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>442</v>
       </c>
@@ -7510,7 +7509,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogteligging</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1">
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>442</v>
       </c>
@@ -7540,7 +7539,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/adrespunt</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1">
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>442</v>
       </c>
@@ -7570,7 +7569,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/eindkap</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1">
+    <row r="133" spans="1:9">
       <c r="A133" t="s">
         <v>442</v>
       </c>
@@ -7600,7 +7599,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/verloopstuk</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1">
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>442</v>
       </c>
@@ -7630,7 +7629,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/afsluiter</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1">
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>442</v>
       </c>
@@ -7660,7 +7659,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/meetpunt</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1">
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>442</v>
       </c>
@@ -7690,7 +7689,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/sifon</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1">
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>442</v>
       </c>
@@ -7720,7 +7719,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/blaasgat</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1">
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>442</v>
       </c>
@@ -7750,7 +7749,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsAppurtenanceIMKLTypeValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1">
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>442</v>
       </c>
@@ -7780,7 +7779,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/gasStation</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1">
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>442</v>
       </c>
@@ -7810,7 +7809,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1">
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>442</v>
       </c>
@@ -7840,7 +7839,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1">
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>442</v>
       </c>
@@ -7870,7 +7869,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1">
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>442</v>
       </c>
@@ -7900,7 +7899,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/productionRegion</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1">
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>442</v>
       </c>
@@ -7930,7 +7929,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pumpingStation</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1">
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>442</v>
       </c>
@@ -7960,7 +7959,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pump</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1">
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>442</v>
       </c>
@@ -7990,7 +7989,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/storage</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1">
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>442</v>
       </c>
@@ -8020,7 +8019,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/terminal</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1">
+    <row r="148" spans="1:9">
       <c r="A148" t="s">
         <v>442</v>
       </c>
@@ -8050,7 +8049,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsProductTypeValue/naturalGas</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1">
+    <row r="149" spans="1:9">
       <c r="A149" t="s">
         <v>442</v>
       </c>
@@ -8080,7 +8079,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductIMKLTypeValue/bioGas</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1">
+    <row r="150" spans="1:9">
       <c r="A150" t="s">
         <v>442</v>
       </c>
@@ -8110,7 +8109,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/accetone</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1">
+    <row r="151" spans="1:9">
       <c r="A151" t="s">
         <v>442</v>
       </c>
@@ -8140,7 +8139,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/air</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1">
+    <row r="152" spans="1:9">
       <c r="A152" t="s">
         <v>442</v>
       </c>
@@ -8170,7 +8169,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/argon</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1">
+    <row r="153" spans="1:9">
       <c r="A153" t="s">
         <v>442</v>
       </c>
@@ -8200,7 +8199,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/butadiene1.2</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1">
+    <row r="154" spans="1:9">
       <c r="A154" t="s">
         <v>442</v>
       </c>
@@ -8230,7 +8229,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/butadiene1.3</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1">
+    <row r="155" spans="1:9">
       <c r="A155" t="s">
         <v>442</v>
       </c>
@@ -8260,7 +8259,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/butane</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1">
+    <row r="156" spans="1:9">
       <c r="A156" t="s">
         <v>442</v>
       </c>
@@ -8290,7 +8289,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/carbonMonoxide</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1">
+    <row r="157" spans="1:9">
       <c r="A157" t="s">
         <v>442</v>
       </c>
@@ -8320,7 +8319,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/chlorine</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1">
+    <row r="158" spans="1:9">
       <c r="A158" t="s">
         <v>442</v>
       </c>
@@ -8350,7 +8349,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/concrete</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1">
+    <row r="159" spans="1:9">
       <c r="A159" t="s">
         <v>442</v>
       </c>
@@ -8380,7 +8379,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/crude</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1">
+    <row r="160" spans="1:9">
       <c r="A160" t="s">
         <v>442</v>
       </c>
@@ -8410,7 +8409,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/dichloroethane</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1">
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>442</v>
       </c>
@@ -8440,7 +8439,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/diesel</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1">
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>442</v>
       </c>
@@ -8470,7 +8469,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/ethylene</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1">
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>442</v>
       </c>
@@ -8500,7 +8499,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/gasFabricationOfCocs</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1">
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>442</v>
       </c>
@@ -8530,7 +8529,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/gasHFx</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1">
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>442</v>
       </c>
@@ -8560,7 +8559,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/gasoil</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1">
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>442</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/hydrogen</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1">
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>442</v>
       </c>
@@ -8620,7 +8619,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/isobutane</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1">
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>442</v>
       </c>
@@ -8650,7 +8649,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/JET-A1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1">
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>442</v>
       </c>
@@ -8680,7 +8679,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/kerosene</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1">
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>442</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/liquidAmmonia</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1">
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>442</v>
       </c>
@@ -8740,7 +8739,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/liquidHydrocarbon</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1">
+    <row r="172" spans="1:9">
       <c r="A172" t="s">
         <v>442</v>
       </c>
@@ -8770,7 +8769,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/multiProduct</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1">
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>442</v>
       </c>
@@ -8800,7 +8799,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/MVC</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1">
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>442</v>
       </c>
@@ -8830,7 +8829,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/nitrogen</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1">
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>442</v>
       </c>
@@ -8860,7 +8859,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/oxygen</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1">
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>442</v>
       </c>
@@ -8890,7 +8889,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/phenol</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1">
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>442</v>
       </c>
@@ -8920,7 +8919,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/propane</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1">
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>442</v>
       </c>
@@ -8950,7 +8949,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/propylene</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1">
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>442</v>
       </c>
@@ -8980,7 +8979,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/saltWater</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1">
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>442</v>
       </c>
@@ -9010,7 +9009,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/saumur</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1">
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>442</v>
       </c>
@@ -9040,7 +9039,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/sand</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1">
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>442</v>
       </c>
@@ -9070,7 +9069,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/tetrachloroide</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1">
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>442</v>
       </c>
@@ -9100,7 +9099,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/unknown</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1">
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>442</v>
       </c>
@@ -9130,7 +9129,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/water</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1">
+    <row r="185" spans="1:9" ht="15" thickBot="1">
       <c r="A185" t="s">
         <v>442</v>
       </c>
@@ -9160,7 +9159,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/OilGasChemicalsProductTypeValue/empty</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="186" spans="1:9" ht="15" thickBot="1">
       <c r="A186" s="4" t="s">
         <v>105</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/afsluiter</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="187" spans="1:9" ht="15" thickBot="1">
       <c r="A187" s="4" t="s">
         <v>105</v>
       </c>
@@ -9220,7 +9219,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/diameterovergang</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="188" spans="1:9" ht="15" thickBot="1">
       <c r="A188" s="4" t="s">
         <v>105</v>
       </c>
@@ -9250,7 +9249,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/materiaalovergang</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="189" spans="1:9" ht="15" thickBot="1">
       <c r="A189" s="4" t="s">
         <v>105</v>
       </c>
@@ -9280,7 +9279,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/eindpunt</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="190" spans="1:9" ht="15" thickBot="1">
       <c r="A190" s="4" t="s">
         <v>105</v>
       </c>
@@ -9310,7 +9309,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/blindflens</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1">
+    <row r="191" spans="1:9">
       <c r="A191" s="4" t="s">
         <v>105</v>
       </c>
@@ -9340,7 +9339,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/airRelieveValve</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1">
+    <row r="192" spans="1:9">
       <c r="A192" s="4" t="s">
         <v>105</v>
       </c>
@@ -9370,7 +9369,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/anode</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1">
+    <row r="193" spans="1:9">
       <c r="A193" s="4" t="s">
         <v>105</v>
       </c>
@@ -9400,7 +9399,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/checkValve</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1">
+    <row r="194" spans="1:9">
       <c r="A194" s="4" t="s">
         <v>105</v>
       </c>
@@ -9430,7 +9429,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/controlValve</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1">
+    <row r="195" spans="1:9">
       <c r="A195" s="4" t="s">
         <v>105</v>
       </c>
@@ -9460,7 +9459,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fireHydrant</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1">
+    <row r="196" spans="1:9">
       <c r="A196" s="4" t="s">
         <v>105</v>
       </c>
@@ -9490,7 +9489,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/junction</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1">
+    <row r="197" spans="1:9">
       <c r="A197" s="4" t="s">
         <v>105</v>
       </c>
@@ -9520,7 +9519,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/lateralPoint</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1">
+    <row r="198" spans="1:9">
       <c r="A198" s="4" t="s">
         <v>105</v>
       </c>
@@ -9550,7 +9549,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/meter</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1">
+    <row r="199" spans="1:9">
       <c r="A199" s="4" t="s">
         <v>105</v>
       </c>
@@ -9580,7 +9579,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pressureController</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1">
+    <row r="200" spans="1:9">
       <c r="A200" s="4" t="s">
         <v>105</v>
       </c>
@@ -9610,7 +9609,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pumpStation</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1">
+    <row r="201" spans="1:9">
       <c r="A201" s="4" t="s">
         <v>105</v>
       </c>
@@ -9640,7 +9639,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/samplingStation</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1">
+    <row r="202" spans="1:9">
       <c r="A202" s="4" t="s">
         <v>105</v>
       </c>
@@ -9670,7 +9669,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/storageFacility</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1">
+    <row r="203" spans="1:9">
       <c r="A203" s="4" t="s">
         <v>105</v>
       </c>
@@ -9700,7 +9699,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/treatmentPlant</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1">
+    <row r="204" spans="1:9">
       <c r="A204" s="4" t="s">
         <v>105</v>
       </c>
@@ -9730,7 +9729,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterDischargePoint</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1">
+    <row r="205" spans="1:9">
       <c r="A205" s="4" t="s">
         <v>105</v>
       </c>
@@ -9760,7 +9759,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterExhaustPoint</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1">
+    <row r="206" spans="1:9">
       <c r="A206" s="4" t="s">
         <v>105</v>
       </c>
@@ -9790,7 +9789,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterServicePoint</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1">
+    <row r="207" spans="1:9">
       <c r="A207" s="4" t="s">
         <v>105</v>
       </c>
@@ -9820,7 +9819,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/well</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="208" spans="1:9" ht="15" thickBot="1">
       <c r="A208" s="4" t="s">
         <v>105</v>
       </c>
@@ -9850,7 +9849,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterTypeValue/industrial</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="209" spans="1:9" ht="15" thickBot="1">
       <c r="A209" s="4" t="s">
         <v>105</v>
       </c>
@@ -9880,7 +9879,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterTypeValue/waste</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1">
+    <row r="210" spans="1:9">
       <c r="A210" s="4" t="s">
         <v>105</v>
       </c>
@@ -9910,7 +9909,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/potable</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1">
+    <row r="211" spans="1:9">
       <c r="A211" s="4" t="s">
         <v>105</v>
       </c>
@@ -9940,7 +9939,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/raw</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1">
+    <row r="212" spans="1:9">
       <c r="A212" s="4" t="s">
         <v>105</v>
       </c>
@@ -9970,7 +9969,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/salt</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1">
+    <row r="213" spans="1:9">
       <c r="A213" s="4" t="s">
         <v>105</v>
       </c>
@@ -10000,7 +9999,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/treated</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="214" spans="1:9" ht="15" thickBot="1">
       <c r="A214" s="4" t="s">
         <v>105</v>
       </c>
@@ -10028,7 +10027,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/WaterAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="215" spans="1:9" ht="15" thickBot="1">
       <c r="A215" s="4" t="s">
         <v>340</v>
       </c>
@@ -10058,7 +10057,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/aansluitleiding</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="216" spans="1:9" ht="15" thickBot="1">
       <c r="A216" s="4" t="s">
         <v>340</v>
       </c>
@@ -10088,7 +10087,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/bergbezinkleiding</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="217" spans="1:9" ht="15" thickBot="1">
       <c r="A217" s="4" t="s">
         <v>340</v>
       </c>
@@ -10118,7 +10117,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/bergingsleiding</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="218" spans="1:9" ht="15" thickBot="1">
       <c r="A218" s="4" t="s">
         <v>340</v>
       </c>
@@ -10148,7 +10147,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/gemengdRiool</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="219" spans="1:9" ht="15" thickBot="1">
       <c r="A219" s="4" t="s">
         <v>340</v>
       </c>
@@ -10178,7 +10177,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/hemelwaterriool</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="220" spans="1:9" ht="15" thickBot="1">
       <c r="A220" s="4" t="s">
         <v>340</v>
       </c>
@@ -10208,7 +10207,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/overstortleiding</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="221" spans="1:9" ht="15" thickBot="1">
       <c r="A221" s="4" t="s">
         <v>340</v>
       </c>
@@ -10238,7 +10237,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/stuwrioolleiding</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="222" spans="1:9" ht="15" thickBot="1">
       <c r="A222" s="4" t="s">
         <v>340</v>
       </c>
@@ -10268,7 +10267,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/doorlatendeleiding</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="223" spans="1:9" ht="15" thickBot="1">
       <c r="A223" s="4" t="s">
         <v>340</v>
       </c>
@@ -10298,7 +10297,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/vuilwaterriool</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="224" spans="1:9" ht="15" thickBot="1">
       <c r="A224" s="4" t="s">
         <v>340</v>
       </c>
@@ -10328,7 +10327,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/transportrioolleiding</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="225" spans="1:9" ht="15" thickBot="1">
       <c r="A225" s="4" t="s">
         <v>340</v>
       </c>
@@ -10358,7 +10357,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/zinker</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="226" spans="1:9" ht="15" thickBot="1">
       <c r="A226" s="4" t="s">
         <v>340</v>
       </c>
@@ -10388,7 +10387,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/RioolleidingTypeValue/openLeiding</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="227" spans="1:9" ht="15" thickBot="1">
       <c r="A227" s="4" t="s">
         <v>340</v>
       </c>
@@ -10418,7 +10417,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/gemaal</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="228" spans="1:9" ht="15" thickBot="1">
       <c r="A228" s="4" t="s">
         <v>340</v>
       </c>
@@ -10448,7 +10447,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/infiltratievoorziening</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="229" spans="1:9" ht="15" thickBot="1">
       <c r="A229" s="4" t="s">
         <v>340</v>
       </c>
@@ -10478,7 +10477,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/kolk</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="15" hidden="1" thickBot="1">
+    <row r="230" spans="1:9" ht="15" thickBot="1">
       <c r="A230" s="4" t="s">
         <v>340</v>
       </c>
@@ -10508,7 +10507,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/kunstwerk</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1">
+    <row r="231" spans="1:9">
       <c r="A231" s="4" t="s">
         <v>340</v>
       </c>
@@ -10538,7 +10537,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/reservoir</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1">
+    <row r="232" spans="1:9">
       <c r="A232" s="4" t="s">
         <v>340</v>
       </c>
@@ -10568,7 +10567,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/uitlaatconstructie</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1">
+    <row r="233" spans="1:9">
       <c r="A233" s="4" t="s">
         <v>340</v>
       </c>
@@ -10598,7 +10597,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/overstort</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1">
+    <row r="234" spans="1:9">
       <c r="A234" s="4" t="s">
         <v>340</v>
       </c>
@@ -10628,7 +10627,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/barrel</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1">
+    <row r="235" spans="1:9">
       <c r="A235" s="4" t="s">
         <v>340</v>
       </c>
@@ -10658,7 +10657,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/catchBasin</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1">
+    <row r="236" spans="1:9">
       <c r="A236" s="4" t="s">
         <v>340</v>
       </c>
@@ -10688,7 +10687,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/cleanOut</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1">
+    <row r="237" spans="1:9">
       <c r="A237" s="4" t="s">
         <v>340</v>
       </c>
@@ -10718,7 +10717,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/connection</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1">
+    <row r="238" spans="1:9">
       <c r="A238" s="4" t="s">
         <v>340</v>
       </c>
@@ -10748,7 +10747,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/dischargeStructure</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1">
+    <row r="239" spans="1:9">
       <c r="A239" s="4" t="s">
         <v>340</v>
       </c>
@@ -10778,7 +10777,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/specificStructure</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1">
+    <row r="240" spans="1:9">
       <c r="A240" s="4" t="s">
         <v>340</v>
       </c>
@@ -10808,7 +10807,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/thrustProtection</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1">
+    <row r="241" spans="1:9">
       <c r="A241" s="4" t="s">
         <v>340</v>
       </c>
@@ -10838,7 +10837,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/tideGate</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1">
+    <row r="242" spans="1:9">
       <c r="A242" s="4" t="s">
         <v>340</v>
       </c>
@@ -10868,7 +10867,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/watertankOrChamber</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1">
+    <row r="243" spans="1:9">
       <c r="A243" s="4" t="s">
         <v>340</v>
       </c>
@@ -10898,7 +10897,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/combined</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1">
+    <row r="244" spans="1:9">
       <c r="A244" s="4" t="s">
         <v>340</v>
       </c>
@@ -10928,7 +10927,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/reclaimed</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1">
+    <row r="245" spans="1:9">
       <c r="A245" s="4" t="s">
         <v>340</v>
       </c>
@@ -10958,7 +10957,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/sanitary</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1">
+    <row r="246" spans="1:9">
       <c r="A246" s="4" t="s">
         <v>340</v>
       </c>
@@ -10988,7 +10987,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/storm</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1">
+    <row r="247" spans="1:9">
       <c r="A247" s="4" t="s">
         <v>340</v>
       </c>
@@ -11015,7 +11014,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/SewerAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="248" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="248" spans="1:9" s="39" customFormat="1">
       <c r="A248" s="46" t="s">
         <v>120</v>
       </c>
@@ -11045,7 +11044,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/compensator</v>
       </c>
     </row>
-    <row r="249" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="249" spans="1:9" s="39" customFormat="1">
       <c r="A249" s="46" t="s">
         <v>120</v>
       </c>
@@ -11075,7 +11074,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/lekdetectiemeetpunt</v>
       </c>
     </row>
-    <row r="250" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="250" spans="1:9" s="39" customFormat="1">
       <c r="A250" s="46" t="s">
         <v>120</v>
       </c>
@@ -11105,7 +11104,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/put</v>
       </c>
     </row>
-    <row r="251" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="251" spans="1:9" s="39" customFormat="1">
       <c r="A251" s="46" t="s">
         <v>120</v>
       </c>
@@ -11135,7 +11134,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/pompstation</v>
       </c>
     </row>
-    <row r="252" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="252" spans="1:9" s="39" customFormat="1">
       <c r="A252" s="46" t="s">
         <v>120</v>
       </c>
@@ -11165,7 +11164,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/overdrachtsstation</v>
       </c>
     </row>
-    <row r="253" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="253" spans="1:9" s="39" customFormat="1">
       <c r="A253" s="46" t="s">
         <v>120</v>
       </c>
@@ -11195,7 +11194,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/mantelbuis</v>
       </c>
     </row>
-    <row r="254" spans="1:9" s="39" customFormat="1" ht="28" hidden="1">
+    <row r="254" spans="1:9" s="39" customFormat="1" ht="28">
       <c r="A254" s="46" t="s">
         <v>120</v>
       </c>
@@ -11225,7 +11224,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/zinker</v>
       </c>
     </row>
-    <row r="255" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="255" spans="1:9" s="39" customFormat="1">
       <c r="A255" s="46" t="s">
         <v>120</v>
       </c>
@@ -11255,7 +11254,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/inEnUittredepuntBoringen</v>
       </c>
     </row>
-    <row r="256" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="256" spans="1:9" s="39" customFormat="1">
       <c r="A256" s="46" t="s">
         <v>120</v>
       </c>
@@ -11285,7 +11284,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/ThermalAppurtenanceTypeIMKLValue/gestuurdeBoring</v>
       </c>
     </row>
-    <row r="257" spans="1:9" s="39" customFormat="1" hidden="1">
+    <row r="257" spans="1:9" s="39" customFormat="1">
       <c r="A257" s="46" t="s">
         <v>120</v>
       </c>
@@ -11878,7 +11877,7 @@
         <v>771</v>
       </c>
       <c r="I278" t="str">
-        <f t="shared" ref="I278:I326" si="4">IF(B278="inspire",INSPIRE,IMKL) &amp; H278 &amp; "/" &amp; E278</f>
+        <f t="shared" ref="I278:I334" si="4">IF(B278="inspire",INSPIRE,IMKL) &amp; H278 &amp; "/" &amp; E278</f>
         <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/RPMP</v>
       </c>
     </row>
@@ -13178,7 +13177,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/HDPE</v>
       </c>
     </row>
-    <row r="327" spans="1:9" hidden="1">
+    <row r="327" spans="1:9">
       <c r="A327" t="s">
         <v>442</v>
       </c>
@@ -13203,8 +13202,12 @@
       <c r="H327" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="328" spans="1:9" hidden="1">
+      <c r="I327" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/31</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9">
       <c r="A328" t="s">
         <v>442</v>
       </c>
@@ -13229,8 +13232,12 @@
       <c r="H328" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="329" spans="1:9" hidden="1">
+      <c r="I328" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/32</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9">
       <c r="A329" t="s">
         <v>442</v>
       </c>
@@ -13255,8 +13262,12 @@
       <c r="H329" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="330" spans="1:9" hidden="1">
+      <c r="I329" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/33</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9">
       <c r="A330" t="s">
         <v>442</v>
       </c>
@@ -13281,8 +13292,12 @@
       <c r="H330" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="331" spans="1:9" hidden="1">
+      <c r="I330" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/34</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9">
       <c r="A331" t="s">
         <v>442</v>
       </c>
@@ -13307,8 +13322,12 @@
       <c r="H331" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="332" spans="1:9" hidden="1">
+      <c r="I331" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/35</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9">
       <c r="A332" t="s">
         <v>442</v>
       </c>
@@ -13333,8 +13352,12 @@
       <c r="H332" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="333" spans="1:9" hidden="1">
+      <c r="I332" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/36</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9">
       <c r="A333" t="s">
         <v>442</v>
       </c>
@@ -13358,6 +13381,10 @@
       </c>
       <c r="H333" t="s">
         <v>704</v>
+      </c>
+      <c r="I333" t="str">
+        <f t="shared" si="4"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/BuisleidingtypeTypeValue/37</v>
       </c>
     </row>
     <row r="334" spans="1:9">
@@ -13386,7 +13413,7 @@
         <v>438</v>
       </c>
       <c r="I334" t="str">
-        <f t="shared" ref="I334:I363" si="5">IF(B334="inspire",INSPIRE,IMKL) &amp; H334 &amp; "/" &amp; E334</f>
+        <f t="shared" si="4"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/waterloop</v>
       </c>
     </row>
@@ -13416,7 +13443,7 @@
         <v>438</v>
       </c>
       <c r="I335" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I334:I363" si="5">IF(B335="inspire",INSPIRE,IMKL) &amp; H335 &amp; "/" &amp; E335</f>
         <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/rijbaan lokale weg</v>
       </c>
     </row>
@@ -14261,13 +14288,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I363">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="algemeen"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState ref="B2:G62">
     <sortCondition ref="D2:D62"/>
     <sortCondition ref="B2:B62"/>

</xml_diff>

<commit_message>
Removing unwanted spaces from codelist values
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.91 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.91 waardelijsten.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="791">
   <si>
     <t>attribuut</t>
   </si>
@@ -2012,9 +2012,6 @@
     <t xml:space="preserve">Chlorinated polyvinyl chloride (CPVC). </t>
   </si>
   <si>
-    <t xml:space="preserve"> FRP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fibre reinforced plastic (FRP). </t>
   </si>
   <si>
@@ -2111,9 +2108,6 @@
     <t>astbestcement</t>
   </si>
   <si>
-    <t xml:space="preserve">BT </t>
-  </si>
-  <si>
     <t>beton</t>
   </si>
   <si>
@@ -2160,9 +2154,6 @@
   </si>
   <si>
     <t xml:space="preserve"> lood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE </t>
   </si>
   <si>
     <t>polyetheen</t>
@@ -2644,6 +2635,21 @@
   </si>
   <si>
     <t>http://www.geonovum.nl/imkl2015/1.0/id/</t>
+  </si>
+  <si>
+    <t>FRP</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>rijbaanLokaleWeg</t>
+  </si>
+  <si>
+    <t>telecomKast</t>
+  </si>
+  <si>
+    <t>CAIkast</t>
   </si>
 </sst>
 </file>
@@ -3591,7 +3597,7 @@
   <sheetData>
     <row r="22" spans="2:3">
       <c r="B22" s="29" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C22" t="s">
         <v>254</v>
@@ -3625,9 +3631,9 @@
   <dimension ref="A1:I363"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I326" sqref="I326:I334"/>
+      <selection pane="bottomLeft" activeCell="E367" sqref="E367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3684,13 +3690,13 @@
         <v>327</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>780</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>783</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>786</v>
-      </c>
       <c r="G2" s="18" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>233</v>
@@ -3714,13 +3720,13 @@
         <v>327</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>781</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>784</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>787</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>233</v>
@@ -3744,13 +3750,13 @@
         <v>327</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>233</v>
@@ -3771,7 +3777,7 @@
         <v>364</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>91</v>
@@ -3801,7 +3807,7 @@
         <v>364</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>92</v>
@@ -3831,7 +3837,7 @@
         <v>364</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>93</v>
@@ -3861,7 +3867,7 @@
         <v>364</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>94</v>
@@ -3891,7 +3897,7 @@
         <v>364</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>338</v>
@@ -3921,7 +3927,7 @@
         <v>364</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>357</v>
@@ -3951,7 +3957,7 @@
         <v>364</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>358</v>
@@ -3981,16 +3987,16 @@
         <v>364</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>359</v>
@@ -4110,7 +4116,7 @@
         <v>462</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>236</v>
@@ -4140,7 +4146,7 @@
         <v>463</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>236</v>
@@ -4170,7 +4176,7 @@
         <v>464</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>236</v>
@@ -4200,7 +4206,7 @@
         <v>87</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>236</v>
@@ -4290,7 +4296,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>237</v>
@@ -4314,13 +4320,13 @@
         <v>326</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" t="str">
@@ -4342,13 +4348,13 @@
         <v>326</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>237</v>
@@ -4378,7 +4384,7 @@
         <v>122</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>237</v>
@@ -4459,19 +4465,19 @@
         <v>364</v>
       </c>
       <c r="D28" s="50" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="E28" s="50" t="s">
+        <v>771</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>775</v>
+      </c>
+      <c r="G28" s="49" t="s">
         <v>774</v>
       </c>
-      <c r="F28" s="50" t="s">
-        <v>778</v>
-      </c>
-      <c r="G28" s="49" t="s">
-        <v>777</v>
-      </c>
       <c r="H28" s="51" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -4489,19 +4495,19 @@
         <v>364</v>
       </c>
       <c r="D29" s="50" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="F29" s="50" t="s">
         <v>397</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -4519,19 +4525,19 @@
         <v>364</v>
       </c>
       <c r="D30" s="50" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="F30" s="50" t="s">
         <v>396</v>
       </c>
       <c r="G30" s="49" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="H30" s="51" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -4549,7 +4555,7 @@
         <v>364</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>84</v>
@@ -4558,7 +4564,7 @@
         <v>84</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>238</v>
@@ -4579,7 +4585,7 @@
         <v>364</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>85</v>
@@ -4588,7 +4594,7 @@
         <v>85</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>238</v>
@@ -4609,7 +4615,7 @@
         <v>364</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>86</v>
@@ -4618,7 +4624,7 @@
         <v>86</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>238</v>
@@ -5089,10 +5095,10 @@
         <v>330</v>
       </c>
       <c r="E49" s="50" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="F49" s="50" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="G49" s="50" t="s">
         <v>455</v>
@@ -5618,13 +5624,13 @@
     <row r="67" spans="1:9">
       <c r="A67" s="1"/>
       <c r="B67" s="18" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>384</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E67" t="s">
         <v>385</v>
@@ -5643,13 +5649,13 @@
     <row r="68" spans="1:9">
       <c r="A68" s="1"/>
       <c r="B68" s="18" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>384</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E68" t="s">
         <v>386</v>
@@ -5668,13 +5674,13 @@
     <row r="69" spans="1:9">
       <c r="A69" s="1"/>
       <c r="B69" s="18" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>384</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E69" t="s">
         <v>387</v>
@@ -5693,13 +5699,13 @@
     <row r="70" spans="1:9">
       <c r="A70" s="1"/>
       <c r="B70" s="18" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>384</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E70" t="s">
         <v>388</v>
@@ -5726,7 +5732,7 @@
         <v>364</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E71" t="s">
         <v>370</v>
@@ -5756,7 +5762,7 @@
         <v>364</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E72" t="s">
         <v>371</v>
@@ -5786,7 +5792,7 @@
         <v>364</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E73" t="s">
         <v>372</v>
@@ -5816,7 +5822,7 @@
         <v>364</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E74" t="s">
         <v>373</v>
@@ -5846,7 +5852,7 @@
         <v>364</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E75" t="s">
         <v>374</v>
@@ -5876,7 +5882,7 @@
         <v>364</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E76" t="s">
         <v>122</v>
@@ -5903,19 +5909,19 @@
         <v>364</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="E77" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="G77" s="31" t="s">
+        <v>705</v>
+      </c>
+      <c r="H77" s="9" t="s">
         <v>707</v>
-      </c>
-      <c r="F77" s="18" t="s">
-        <v>707</v>
-      </c>
-      <c r="G77" s="31" t="s">
-        <v>708</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>710</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="0"/>
@@ -5933,19 +5939,19 @@
         <v>364</v>
       </c>
       <c r="D78" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="E78" s="18" t="s">
         <v>706</v>
       </c>
-      <c r="E78" s="18" t="s">
-        <v>709</v>
-      </c>
       <c r="F78" s="18" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="G78" s="31" t="s">
         <v>395</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="I78" t="str">
         <f t="shared" si="0"/>
@@ -6596,13 +6602,13 @@
         <v>320</v>
       </c>
       <c r="E100" s="40" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="F100" s="40" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="G100" s="40" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="H100" s="42" t="s">
         <v>244</v>
@@ -6686,13 +6692,13 @@
         <v>320</v>
       </c>
       <c r="E103" s="40" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="F103" s="40" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="G103" s="40" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="H103" s="42" t="s">
         <v>244</v>
@@ -7766,7 +7772,7 @@
         <v>299</v>
       </c>
       <c r="F139" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="G139" t="s">
         <v>32</v>
@@ -7796,7 +7802,7 @@
         <v>300</v>
       </c>
       <c r="F140" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="G140" t="s">
         <v>36</v>
@@ -10035,10 +10041,10 @@
         <v>193</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E215" s="24" t="s">
         <v>398</v>
@@ -10050,7 +10056,7 @@
         <v>398</v>
       </c>
       <c r="H215" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I215" t="str">
         <f t="shared" si="3"/>
@@ -10065,10 +10071,10 @@
         <v>193</v>
       </c>
       <c r="C216" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E216" s="24" t="s">
         <v>399</v>
@@ -10080,7 +10086,7 @@
         <v>399</v>
       </c>
       <c r="H216" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I216" t="str">
         <f t="shared" si="3"/>
@@ -10095,10 +10101,10 @@
         <v>193</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E217" s="24" t="s">
         <v>400</v>
@@ -10110,7 +10116,7 @@
         <v>400</v>
       </c>
       <c r="H217" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I217" t="str">
         <f t="shared" si="3"/>
@@ -10125,10 +10131,10 @@
         <v>193</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E218" s="24" t="s">
         <v>401</v>
@@ -10140,7 +10146,7 @@
         <v>474</v>
       </c>
       <c r="H218" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I218" t="str">
         <f t="shared" si="3"/>
@@ -10155,10 +10161,10 @@
         <v>193</v>
       </c>
       <c r="C219" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E219" s="24" t="s">
         <v>402</v>
@@ -10170,7 +10176,7 @@
         <v>402</v>
       </c>
       <c r="H219" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I219" t="str">
         <f t="shared" si="3"/>
@@ -10185,10 +10191,10 @@
         <v>193</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E220" s="24" t="s">
         <v>403</v>
@@ -10200,7 +10206,7 @@
         <v>403</v>
       </c>
       <c r="H220" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I220" t="str">
         <f t="shared" si="3"/>
@@ -10215,10 +10221,10 @@
         <v>193</v>
       </c>
       <c r="C221" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E221" s="24" t="s">
         <v>404</v>
@@ -10230,7 +10236,7 @@
         <v>404</v>
       </c>
       <c r="H221" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I221" t="str">
         <f t="shared" si="3"/>
@@ -10245,10 +10251,10 @@
         <v>193</v>
       </c>
       <c r="C222" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E222" s="24" t="s">
         <v>405</v>
@@ -10260,7 +10266,7 @@
         <v>405</v>
       </c>
       <c r="H222" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I222" t="str">
         <f t="shared" si="3"/>
@@ -10275,10 +10281,10 @@
         <v>193</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E223" s="24" t="s">
         <v>406</v>
@@ -10290,7 +10296,7 @@
         <v>406</v>
       </c>
       <c r="H223" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I223" t="str">
         <f t="shared" si="3"/>
@@ -10305,10 +10311,10 @@
         <v>193</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E224" s="24" t="s">
         <v>407</v>
@@ -10320,7 +10326,7 @@
         <v>407</v>
       </c>
       <c r="H224" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I224" t="str">
         <f t="shared" si="3"/>
@@ -10335,10 +10341,10 @@
         <v>193</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E225" s="24" t="s">
         <v>316</v>
@@ -10350,7 +10356,7 @@
         <v>316</v>
       </c>
       <c r="H225" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I225" t="str">
         <f t="shared" si="3"/>
@@ -10365,10 +10371,10 @@
         <v>193</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E226" s="24" t="s">
         <v>408</v>
@@ -10380,7 +10386,7 @@
         <v>408</v>
       </c>
       <c r="H226" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I226" t="str">
         <f t="shared" si="3"/>
@@ -11325,7 +11331,7 @@
         <v>560</v>
       </c>
       <c r="D258" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E258" s="18" t="s">
         <v>561</v>
@@ -11334,7 +11340,7 @@
         <v>562</v>
       </c>
       <c r="H258" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I258" t="str">
         <f t="shared" si="3"/>
@@ -11352,7 +11358,7 @@
         <v>560</v>
       </c>
       <c r="D259" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E259" s="8" t="s">
         <v>563</v>
@@ -11361,7 +11367,7 @@
         <v>564</v>
       </c>
       <c r="H259" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I259" t="str">
         <f t="shared" si="3"/>
@@ -11379,7 +11385,7 @@
         <v>560</v>
       </c>
       <c r="D260" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E260" s="8" t="s">
         <v>565</v>
@@ -11388,7 +11394,7 @@
         <v>566</v>
       </c>
       <c r="H260" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I260" t="str">
         <f t="shared" si="3"/>
@@ -11406,7 +11412,7 @@
         <v>560</v>
       </c>
       <c r="D261" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E261" s="8" t="s">
         <v>567</v>
@@ -11415,7 +11421,7 @@
         <v>568</v>
       </c>
       <c r="H261" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I261" t="str">
         <f t="shared" si="3"/>
@@ -11433,7 +11439,7 @@
         <v>560</v>
       </c>
       <c r="D262" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E262" s="8" t="s">
         <v>569</v>
@@ -11442,7 +11448,7 @@
         <v>570</v>
       </c>
       <c r="H262" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I262" t="str">
         <f t="shared" si="3"/>
@@ -11460,7 +11466,7 @@
         <v>560</v>
       </c>
       <c r="D263" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E263" s="8" t="s">
         <v>571</v>
@@ -11469,7 +11475,7 @@
         <v>572</v>
       </c>
       <c r="H263" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I263" t="str">
         <f t="shared" si="3"/>
@@ -11487,7 +11493,7 @@
         <v>560</v>
       </c>
       <c r="D264" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E264" s="8" t="s">
         <v>573</v>
@@ -11496,7 +11502,7 @@
         <v>574</v>
       </c>
       <c r="H264" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I264" t="str">
         <f t="shared" si="3"/>
@@ -11514,7 +11520,7 @@
         <v>560</v>
       </c>
       <c r="D265" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E265" s="8" t="s">
         <v>138</v>
@@ -11523,7 +11529,7 @@
         <v>575</v>
       </c>
       <c r="H265" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I265" t="str">
         <f t="shared" si="3"/>
@@ -11541,7 +11547,7 @@
         <v>560</v>
       </c>
       <c r="D266" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E266" s="8" t="s">
         <v>576</v>
@@ -11550,7 +11556,7 @@
         <v>577</v>
       </c>
       <c r="H266" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I266" t="str">
         <f t="shared" si="3"/>
@@ -11568,20 +11574,20 @@
         <v>560</v>
       </c>
       <c r="D267" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E267" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="G267" t="s">
         <v>578</v>
       </c>
-      <c r="G267" t="s">
-        <v>579</v>
-      </c>
       <c r="H267" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I267" t="str">
         <f t="shared" si="3"/>
-        <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/ FRP</v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/FRP</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -11595,16 +11601,16 @@
         <v>560</v>
       </c>
       <c r="D268" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E268" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="G268" t="s">
         <v>580</v>
       </c>
-      <c r="G268" t="s">
-        <v>581</v>
-      </c>
       <c r="H268" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I268" t="str">
         <f t="shared" si="3"/>
@@ -11622,16 +11628,16 @@
         <v>560</v>
       </c>
       <c r="D269" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E269" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="G269" t="s">
         <v>582</v>
       </c>
-      <c r="G269" t="s">
-        <v>583</v>
-      </c>
       <c r="H269" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I269" t="str">
         <f t="shared" si="3"/>
@@ -11649,16 +11655,16 @@
         <v>560</v>
       </c>
       <c r="D270" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E270" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="G270" t="s">
         <v>584</v>
       </c>
-      <c r="G270" t="s">
-        <v>585</v>
-      </c>
       <c r="H270" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I270" t="str">
         <f t="shared" si="3"/>
@@ -11676,16 +11682,16 @@
         <v>560</v>
       </c>
       <c r="D271" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E271" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="G271" t="s">
         <v>586</v>
       </c>
-      <c r="G271" t="s">
-        <v>587</v>
-      </c>
       <c r="H271" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I271" t="str">
         <f t="shared" si="3"/>
@@ -11703,16 +11709,16 @@
         <v>560</v>
       </c>
       <c r="D272" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E272" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="G272" t="s">
         <v>588</v>
       </c>
-      <c r="G272" t="s">
-        <v>589</v>
-      </c>
       <c r="H272" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I272" t="str">
         <f t="shared" si="3"/>
@@ -11730,16 +11736,16 @@
         <v>560</v>
       </c>
       <c r="D273" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E273" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="G273" t="s">
         <v>590</v>
       </c>
-      <c r="G273" t="s">
-        <v>591</v>
-      </c>
       <c r="H273" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I273" t="str">
         <f t="shared" si="3"/>
@@ -11757,16 +11763,16 @@
         <v>560</v>
       </c>
       <c r="D274" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E274" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="G274" t="s">
         <v>592</v>
       </c>
-      <c r="G274" t="s">
-        <v>593</v>
-      </c>
       <c r="H274" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I274" t="str">
         <f t="shared" si="3"/>
@@ -11784,16 +11790,16 @@
         <v>560</v>
       </c>
       <c r="D275" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E275" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="G275" t="s">
         <v>594</v>
       </c>
-      <c r="G275" t="s">
-        <v>595</v>
-      </c>
       <c r="H275" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I275" t="str">
         <f t="shared" si="3"/>
@@ -11811,16 +11817,16 @@
         <v>560</v>
       </c>
       <c r="D276" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E276" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="G276" t="s">
         <v>596</v>
       </c>
-      <c r="G276" t="s">
-        <v>597</v>
-      </c>
       <c r="H276" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I276" t="str">
         <f t="shared" si="3"/>
@@ -11838,16 +11844,16 @@
         <v>560</v>
       </c>
       <c r="D277" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E277" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="G277" t="s">
         <v>598</v>
       </c>
-      <c r="G277" t="s">
-        <v>599</v>
-      </c>
       <c r="H277" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I277" t="str">
         <f t="shared" si="3"/>
@@ -11865,16 +11871,16 @@
         <v>560</v>
       </c>
       <c r="D278" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E278" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="G278" t="s">
         <v>600</v>
       </c>
-      <c r="G278" t="s">
-        <v>601</v>
-      </c>
       <c r="H278" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I278" t="str">
         <f t="shared" ref="I278:I334" si="4">IF(B278="inspire",INSPIRE,IMKL) &amp; H278 &amp; "/" &amp; E278</f>
@@ -11892,16 +11898,16 @@
         <v>560</v>
       </c>
       <c r="D279" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E279" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="G279" t="s">
         <v>602</v>
       </c>
-      <c r="G279" t="s">
-        <v>603</v>
-      </c>
       <c r="H279" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I279" t="str">
         <f t="shared" si="4"/>
@@ -11919,16 +11925,16 @@
         <v>560</v>
       </c>
       <c r="D280" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E280" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="G280" t="s">
         <v>604</v>
       </c>
-      <c r="G280" t="s">
-        <v>605</v>
-      </c>
       <c r="H280" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I280" t="str">
         <f t="shared" si="4"/>
@@ -11946,16 +11952,16 @@
         <v>560</v>
       </c>
       <c r="D281" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E281" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="G281" t="s">
         <v>606</v>
       </c>
-      <c r="G281" t="s">
-        <v>607</v>
-      </c>
       <c r="H281" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I281" t="str">
         <f t="shared" si="4"/>
@@ -11967,22 +11973,22 @@
         <v>338</v>
       </c>
       <c r="B282" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C282" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D282" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E282" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="G282" s="34" t="s">
         <v>609</v>
       </c>
-      <c r="G282" s="34" t="s">
-        <v>610</v>
-      </c>
       <c r="H282" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I282" t="str">
         <f t="shared" si="4"/>
@@ -11994,26 +12000,26 @@
         <v>338</v>
       </c>
       <c r="B283" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C283" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D283" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E283" s="8" t="s">
-        <v>611</v>
+        <v>787</v>
       </c>
       <c r="G283" s="34" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H283" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I283" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/BT </v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/BT</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -12021,22 +12027,22 @@
         <v>338</v>
       </c>
       <c r="B284" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C284" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D284" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E284" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="G284" s="34" t="s">
         <v>613</v>
       </c>
-      <c r="G284" s="34" t="s">
-        <v>615</v>
-      </c>
       <c r="H284" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I284" t="str">
         <f t="shared" si="4"/>
@@ -12048,22 +12054,22 @@
         <v>338</v>
       </c>
       <c r="B285" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C285" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D285" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="G285" s="34" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H285" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I285" t="str">
         <f t="shared" si="4"/>
@@ -12075,22 +12081,22 @@
         <v>338</v>
       </c>
       <c r="B286" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C286" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D286" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G286" s="34" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H286" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I286" t="str">
         <f t="shared" si="4"/>
@@ -12102,22 +12108,22 @@
         <v>338</v>
       </c>
       <c r="B287" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C287" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D287" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E287" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G287" s="34" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H287" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I287" t="str">
         <f t="shared" si="4"/>
@@ -12129,22 +12135,22 @@
         <v>338</v>
       </c>
       <c r="B288" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C288" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D288" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E288" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="G288" s="34" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H288" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I288" t="str">
         <f t="shared" si="4"/>
@@ -12156,22 +12162,22 @@
         <v>338</v>
       </c>
       <c r="B289" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C289" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D289" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E289" s="8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G289" s="34" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H289" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I289" t="str">
         <f t="shared" si="4"/>
@@ -12183,22 +12189,22 @@
         <v>338</v>
       </c>
       <c r="B290" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C290" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D290" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E290" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G290" s="34" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H290" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I290" t="str">
         <f t="shared" si="4"/>
@@ -12210,22 +12216,22 @@
         <v>338</v>
       </c>
       <c r="B291" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C291" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D291" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E291" s="8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G291" s="34" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H291" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I291" t="str">
         <f t="shared" si="4"/>
@@ -12237,26 +12243,26 @@
         <v>338</v>
       </c>
       <c r="B292" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C292" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D292" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E292" s="8" t="s">
-        <v>628</v>
+        <v>587</v>
       </c>
       <c r="G292" s="34" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="H292" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I292" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/PE </v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/PipeMaterialTypeValue/PE</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -12264,22 +12270,22 @@
         <v>338</v>
       </c>
       <c r="B293" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C293" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D293" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E293" s="8" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="G293" s="34" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="H293" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I293" t="str">
         <f t="shared" si="4"/>
@@ -12291,22 +12297,22 @@
         <v>338</v>
       </c>
       <c r="B294" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C294" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D294" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E294" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G294" s="34" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="H294" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I294" t="str">
         <f t="shared" si="4"/>
@@ -12318,22 +12324,22 @@
         <v>338</v>
       </c>
       <c r="B295" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C295" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D295" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E295" s="8" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="G295" s="34" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="H295" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I295" t="str">
         <f t="shared" si="4"/>
@@ -12345,22 +12351,22 @@
         <v>338</v>
       </c>
       <c r="B296" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C296" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D296" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E296" s="8" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="G296" s="34" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="H296" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I296" t="str">
         <f t="shared" si="4"/>
@@ -12372,22 +12378,22 @@
         <v>338</v>
       </c>
       <c r="B297" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C297" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D297" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="G297" s="34" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="H297" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I297" t="str">
         <f t="shared" si="4"/>
@@ -12399,22 +12405,22 @@
         <v>338</v>
       </c>
       <c r="B298" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C298" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D298" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="G298" s="34" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="H298" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I298" t="str">
         <f t="shared" si="4"/>
@@ -12426,22 +12432,22 @@
         <v>338</v>
       </c>
       <c r="B299" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C299" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D299" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E299" s="8" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="G299" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="H299" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I299" t="str">
         <f t="shared" si="4"/>
@@ -12453,22 +12459,22 @@
         <v>338</v>
       </c>
       <c r="B300" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C300" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D300" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E300" s="8" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G300" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="H300" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I300" t="str">
         <f t="shared" si="4"/>
@@ -12480,22 +12486,22 @@
         <v>338</v>
       </c>
       <c r="B301" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C301" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D301" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E301" s="8" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="G301" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="H301" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I301" t="str">
         <f t="shared" si="4"/>
@@ -12507,22 +12513,22 @@
         <v>338</v>
       </c>
       <c r="B302" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C302" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D302" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E302" s="8" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="G302" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="H302" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I302" t="str">
         <f t="shared" si="4"/>
@@ -12534,22 +12540,22 @@
         <v>338</v>
       </c>
       <c r="B303" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C303" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D303" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E303" s="8" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G303" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="H303" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I303" t="str">
         <f t="shared" si="4"/>
@@ -12561,22 +12567,22 @@
         <v>338</v>
       </c>
       <c r="B304" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C304" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D304" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E304" s="8" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="G304" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="H304" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I304" t="str">
         <f t="shared" si="4"/>
@@ -12588,22 +12594,22 @@
         <v>338</v>
       </c>
       <c r="B305" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C305" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D305" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E305" s="8" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="G305" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="H305" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I305" t="str">
         <f t="shared" si="4"/>
@@ -12615,22 +12621,22 @@
         <v>338</v>
       </c>
       <c r="B306" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C306" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D306" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E306" s="8" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="G306" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="H306" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I306" t="str">
         <f t="shared" si="4"/>
@@ -12642,22 +12648,22 @@
         <v>338</v>
       </c>
       <c r="B307" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C307" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D307" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E307" s="8" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="G307" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="H307" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I307" t="str">
         <f t="shared" si="4"/>
@@ -12669,22 +12675,22 @@
         <v>338</v>
       </c>
       <c r="B308" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C308" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D308" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E308" s="8" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G308" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="H308" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I308" t="str">
         <f t="shared" si="4"/>
@@ -12696,22 +12702,22 @@
         <v>338</v>
       </c>
       <c r="B309" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C309" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D309" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E309" s="8" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="G309" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H309" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I309" t="str">
         <f t="shared" si="4"/>
@@ -12723,22 +12729,22 @@
         <v>338</v>
       </c>
       <c r="B310" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C310" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D310" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E310" s="8" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G310" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="H310" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I310" t="str">
         <f t="shared" si="4"/>
@@ -12750,22 +12756,22 @@
         <v>338</v>
       </c>
       <c r="B311" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C311" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D311" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E311" s="8" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="G311" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="H311" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I311" t="str">
         <f t="shared" si="4"/>
@@ -12777,22 +12783,22 @@
         <v>338</v>
       </c>
       <c r="B312" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C312" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D312" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E312" s="8" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="G312" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="H312" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I312" t="str">
         <f t="shared" si="4"/>
@@ -12804,22 +12810,22 @@
         <v>338</v>
       </c>
       <c r="B313" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C313" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D313" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E313" s="8" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="G313" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="H313" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I313" t="str">
         <f t="shared" si="4"/>
@@ -12831,22 +12837,22 @@
         <v>338</v>
       </c>
       <c r="B314" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C314" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D314" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E314" s="8" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G314" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="H314" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I314" t="str">
         <f t="shared" si="4"/>
@@ -12858,22 +12864,22 @@
         <v>338</v>
       </c>
       <c r="B315" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C315" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D315" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E315" s="8" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="G315" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="H315" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I315" t="str">
         <f t="shared" si="4"/>
@@ -12885,22 +12891,22 @@
         <v>338</v>
       </c>
       <c r="B316" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C316" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D316" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E316" s="8" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="G316" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="H316" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I316" t="str">
         <f t="shared" si="4"/>
@@ -12912,22 +12918,22 @@
         <v>338</v>
       </c>
       <c r="B317" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C317" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D317" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E317" s="8" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="G317" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="H317" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I317" t="str">
         <f t="shared" si="4"/>
@@ -12939,22 +12945,22 @@
         <v>338</v>
       </c>
       <c r="B318" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C318" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D318" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E318" s="8" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="G318" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H318" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I318" t="str">
         <f t="shared" si="4"/>
@@ -12966,22 +12972,22 @@
         <v>338</v>
       </c>
       <c r="B319" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C319" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D319" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E319" s="8" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="G319" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="H319" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I319" t="str">
         <f t="shared" si="4"/>
@@ -12993,22 +12999,22 @@
         <v>338</v>
       </c>
       <c r="B320" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C320" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D320" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E320" s="8" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="G320" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="H320" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I320" t="str">
         <f t="shared" si="4"/>
@@ -13020,22 +13026,22 @@
         <v>338</v>
       </c>
       <c r="B321" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C321" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D321" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E321" s="8" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="G321" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="H321" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I321" t="str">
         <f t="shared" si="4"/>
@@ -13047,22 +13053,22 @@
         <v>338</v>
       </c>
       <c r="B322" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C322" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D322" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E322" s="8" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="G322" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="H322" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I322" t="str">
         <f t="shared" si="4"/>
@@ -13074,22 +13080,22 @@
         <v>338</v>
       </c>
       <c r="B323" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C323" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D323" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E323" s="8" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="G323" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="H323" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I323" t="str">
         <f t="shared" si="4"/>
@@ -13101,22 +13107,22 @@
         <v>338</v>
       </c>
       <c r="B324" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C324" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D324" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E324" s="8" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="G324" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="H324" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I324" t="str">
         <f t="shared" si="4"/>
@@ -13128,22 +13134,22 @@
         <v>338</v>
       </c>
       <c r="B325" s="18" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C325" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D325" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E325" s="8" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="G325" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="H325" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I325" t="str">
         <f t="shared" si="4"/>
@@ -13155,22 +13161,22 @@
         <v>338</v>
       </c>
       <c r="B326" s="18" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C326" s="18" t="s">
         <v>560</v>
       </c>
       <c r="D326" s="18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E326" s="8" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G326" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="H326" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I326" t="str">
         <f t="shared" si="4"/>
@@ -13182,25 +13188,25 @@
         <v>442</v>
       </c>
       <c r="B327" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C327" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D327" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E327" s="36">
         <v>31</v>
       </c>
       <c r="F327" s="35" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="G327" s="35" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="H327" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I327" t="str">
         <f t="shared" si="4"/>
@@ -13212,13 +13218,13 @@
         <v>442</v>
       </c>
       <c r="B328" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C328" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D328" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E328" s="37">
         <v>32</v>
@@ -13230,7 +13236,7 @@
         <v>366</v>
       </c>
       <c r="H328" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I328" t="str">
         <f t="shared" si="4"/>
@@ -13242,13 +13248,13 @@
         <v>442</v>
       </c>
       <c r="B329" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C329" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D329" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E329" s="37">
         <v>33</v>
@@ -13260,7 +13266,7 @@
         <v>367</v>
       </c>
       <c r="H329" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I329" t="str">
         <f t="shared" si="4"/>
@@ -13272,13 +13278,13 @@
         <v>442</v>
       </c>
       <c r="B330" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C330" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D330" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E330" s="37">
         <v>34</v>
@@ -13290,7 +13296,7 @@
         <v>368</v>
       </c>
       <c r="H330" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I330" t="str">
         <f t="shared" si="4"/>
@@ -13302,13 +13308,13 @@
         <v>442</v>
       </c>
       <c r="B331" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C331" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D331" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E331" s="37">
         <v>35</v>
@@ -13320,7 +13326,7 @@
         <v>369</v>
       </c>
       <c r="H331" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I331" t="str">
         <f t="shared" si="4"/>
@@ -13332,13 +13338,13 @@
         <v>442</v>
       </c>
       <c r="B332" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C332" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D332" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E332" s="37">
         <v>36</v>
@@ -13350,7 +13356,7 @@
         <v>122</v>
       </c>
       <c r="H332" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I332" t="str">
         <f t="shared" si="4"/>
@@ -13362,25 +13368,25 @@
         <v>442</v>
       </c>
       <c r="B333" s="35" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C333" s="18" t="s">
         <v>384</v>
       </c>
       <c r="D333" s="35" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E333" s="37">
         <v>37</v>
       </c>
       <c r="F333" t="s">
+        <v>698</v>
+      </c>
+      <c r="G333" t="s">
+        <v>698</v>
+      </c>
+      <c r="H333" t="s">
         <v>701</v>
-      </c>
-      <c r="G333" t="s">
-        <v>701</v>
-      </c>
-      <c r="H333" t="s">
-        <v>704</v>
       </c>
       <c r="I333" t="str">
         <f t="shared" si="4"/>
@@ -13392,13 +13398,13 @@
         <v>338</v>
       </c>
       <c r="B334" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C334" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D334" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E334" t="s">
         <v>411</v>
@@ -13407,7 +13413,7 @@
         <v>411</v>
       </c>
       <c r="G334" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="H334" s="9" t="s">
         <v>438</v>
@@ -13422,29 +13428,29 @@
         <v>338</v>
       </c>
       <c r="B335" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C335" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D335" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E335" t="s">
-        <v>412</v>
+        <v>788</v>
       </c>
       <c r="F335" t="s">
         <v>412</v>
       </c>
       <c r="G335" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="H335" s="9" t="s">
         <v>438</v>
       </c>
       <c r="I335" t="str">
-        <f t="shared" ref="I334:I363" si="5">IF(B335="inspire",INSPIRE,IMKL) &amp; H335 &amp; "/" &amp; E335</f>
-        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/rijbaan lokale weg</v>
+        <f t="shared" ref="I335:I363" si="5">IF(B335="inspire",INSPIRE,IMKL) &amp; H335 &amp; "/" &amp; E335</f>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/rijbaanLokaleWeg</v>
       </c>
     </row>
     <row r="336" spans="1:9">
@@ -13452,13 +13458,13 @@
         <v>338</v>
       </c>
       <c r="B336" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C336" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D336" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E336" t="s">
         <v>413</v>
@@ -13467,7 +13473,7 @@
         <v>413</v>
       </c>
       <c r="G336" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="H336" s="9" t="s">
         <v>438</v>
@@ -13482,13 +13488,13 @@
         <v>338</v>
       </c>
       <c r="B337" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C337" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D337" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E337" t="s">
         <v>414</v>
@@ -13497,7 +13503,7 @@
         <v>414</v>
       </c>
       <c r="G337" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="H337" s="9" t="s">
         <v>438</v>
@@ -13512,13 +13518,13 @@
         <v>338</v>
       </c>
       <c r="B338" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C338" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D338" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E338" t="s">
         <v>415</v>
@@ -13527,7 +13533,7 @@
         <v>415</v>
       </c>
       <c r="G338" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="H338" s="9" t="s">
         <v>438</v>
@@ -13542,13 +13548,13 @@
         <v>338</v>
       </c>
       <c r="B339" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C339" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D339" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E339" t="s">
         <v>439</v>
@@ -13557,7 +13563,7 @@
         <v>416</v>
       </c>
       <c r="G339" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="H339" s="9" t="s">
         <v>438</v>
@@ -13572,22 +13578,22 @@
         <v>338</v>
       </c>
       <c r="B340" s="41" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C340" s="41" t="s">
         <v>364</v>
       </c>
       <c r="D340" s="41" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E340" s="39" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="F340" s="39" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="G340" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="H340" s="44" t="s">
         <v>438</v>
@@ -13602,13 +13608,13 @@
         <v>338</v>
       </c>
       <c r="B341" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C341" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D341" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E341" t="s">
         <v>417</v>
@@ -13617,7 +13623,7 @@
         <v>417</v>
       </c>
       <c r="G341" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="H341" s="9" t="s">
         <v>438</v>
@@ -13632,13 +13638,13 @@
         <v>338</v>
       </c>
       <c r="B342" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C342" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D342" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E342" t="s">
         <v>418</v>
@@ -13647,7 +13653,7 @@
         <v>418</v>
       </c>
       <c r="G342" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="H342" s="9" t="s">
         <v>438</v>
@@ -13662,13 +13668,13 @@
         <v>338</v>
       </c>
       <c r="B343" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C343" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D343" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E343" t="s">
         <v>419</v>
@@ -13677,7 +13683,7 @@
         <v>419</v>
       </c>
       <c r="G343" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="H343" s="9" t="s">
         <v>438</v>
@@ -13692,13 +13698,13 @@
         <v>338</v>
       </c>
       <c r="B344" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C344" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D344" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E344" t="s">
         <v>420</v>
@@ -13707,7 +13713,7 @@
         <v>420</v>
       </c>
       <c r="G344" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="H344" s="9" t="s">
         <v>438</v>
@@ -13722,13 +13728,13 @@
         <v>338</v>
       </c>
       <c r="B345" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C345" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D345" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E345" t="s">
         <v>421</v>
@@ -13737,7 +13743,7 @@
         <v>421</v>
       </c>
       <c r="G345" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="H345" s="9" t="s">
         <v>438</v>
@@ -13752,13 +13758,13 @@
         <v>338</v>
       </c>
       <c r="B346" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C346" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D346" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E346" t="s">
         <v>422</v>
@@ -13767,7 +13773,7 @@
         <v>422</v>
       </c>
       <c r="G346" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="H346" s="9" t="s">
         <v>438</v>
@@ -13782,13 +13788,13 @@
         <v>338</v>
       </c>
       <c r="B347" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C347" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D347" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E347" t="s">
         <v>423</v>
@@ -13797,7 +13803,7 @@
         <v>423</v>
       </c>
       <c r="G347" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="H347" s="9" t="s">
         <v>438</v>
@@ -13812,13 +13818,13 @@
         <v>338</v>
       </c>
       <c r="B348" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C348" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D348" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E348" t="s">
         <v>424</v>
@@ -13827,7 +13833,7 @@
         <v>424</v>
       </c>
       <c r="G348" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="H348" s="9" t="s">
         <v>438</v>
@@ -13842,13 +13848,13 @@
         <v>338</v>
       </c>
       <c r="B349" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C349" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D349" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E349" t="s">
         <v>425</v>
@@ -13857,7 +13863,7 @@
         <v>425</v>
       </c>
       <c r="G349" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="H349" s="9" t="s">
         <v>438</v>
@@ -13872,13 +13878,13 @@
         <v>338</v>
       </c>
       <c r="B350" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C350" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D350" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E350" t="s">
         <v>187</v>
@@ -13887,7 +13893,7 @@
         <v>187</v>
       </c>
       <c r="G350" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="H350" s="9" t="s">
         <v>438</v>
@@ -13902,13 +13908,13 @@
         <v>338</v>
       </c>
       <c r="B351" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C351" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D351" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E351" t="s">
         <v>426</v>
@@ -13917,7 +13923,7 @@
         <v>426</v>
       </c>
       <c r="G351" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="H351" s="9" t="s">
         <v>438</v>
@@ -13932,13 +13938,13 @@
         <v>338</v>
       </c>
       <c r="B352" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C352" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D352" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E352" t="s">
         <v>427</v>
@@ -13947,7 +13953,7 @@
         <v>427</v>
       </c>
       <c r="G352" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H352" s="9" t="s">
         <v>438</v>
@@ -13962,29 +13968,29 @@
         <v>338</v>
       </c>
       <c r="B353" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C353" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D353" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E353" t="s">
-        <v>428</v>
+        <v>790</v>
       </c>
       <c r="F353" t="s">
         <v>428</v>
       </c>
       <c r="G353" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="H353" s="9" t="s">
         <v>438</v>
       </c>
       <c r="I353" t="str">
         <f t="shared" si="5"/>
-        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/CAI-kast</v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/CAIkast</v>
       </c>
     </row>
     <row r="354" spans="1:9">
@@ -13992,13 +13998,13 @@
         <v>338</v>
       </c>
       <c r="B354" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C354" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D354" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E354" t="s">
         <v>429</v>
@@ -14007,7 +14013,7 @@
         <v>429</v>
       </c>
       <c r="G354" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="H354" s="9" t="s">
         <v>438</v>
@@ -14022,13 +14028,13 @@
         <v>338</v>
       </c>
       <c r="B355" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C355" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D355" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E355" t="s">
         <v>430</v>
@@ -14037,7 +14043,7 @@
         <v>430</v>
       </c>
       <c r="G355" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="H355" s="9" t="s">
         <v>438</v>
@@ -14052,29 +14058,29 @@
         <v>338</v>
       </c>
       <c r="B356" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C356" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D356" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E356" t="s">
-        <v>431</v>
+        <v>789</v>
       </c>
       <c r="F356" t="s">
         <v>431</v>
       </c>
       <c r="G356" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="H356" s="9" t="s">
         <v>438</v>
       </c>
       <c r="I356" t="str">
         <f t="shared" si="5"/>
-        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/telecom kast</v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/id/TopografischObjectTypeValue/telecomKast</v>
       </c>
     </row>
     <row r="357" spans="1:9">
@@ -14082,13 +14088,13 @@
         <v>338</v>
       </c>
       <c r="B357" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C357" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D357" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E357" t="s">
         <v>432</v>
@@ -14097,7 +14103,7 @@
         <v>432</v>
       </c>
       <c r="G357" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="H357" s="9" t="s">
         <v>438</v>
@@ -14112,22 +14118,22 @@
         <v>338</v>
       </c>
       <c r="B358" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C358" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D358" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E358" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="F358" t="s">
         <v>433</v>
       </c>
       <c r="G358" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="H358" s="9" t="s">
         <v>438</v>
@@ -14142,13 +14148,13 @@
         <v>338</v>
       </c>
       <c r="B359" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C359" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D359" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E359" t="s">
         <v>434</v>
@@ -14157,7 +14163,7 @@
         <v>434</v>
       </c>
       <c r="G359" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="H359" s="9" t="s">
         <v>438</v>
@@ -14172,13 +14178,13 @@
         <v>338</v>
       </c>
       <c r="B360" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C360" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D360" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E360" t="s">
         <v>435</v>
@@ -14187,7 +14193,7 @@
         <v>435</v>
       </c>
       <c r="G360" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="H360" s="9" t="s">
         <v>438</v>
@@ -14202,13 +14208,13 @@
         <v>338</v>
       </c>
       <c r="B361" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C361" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D361" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E361" t="s">
         <v>436</v>
@@ -14217,7 +14223,7 @@
         <v>436</v>
       </c>
       <c r="G361" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="H361" s="9" t="s">
         <v>438</v>
@@ -14232,13 +14238,13 @@
         <v>338</v>
       </c>
       <c r="B362" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C362" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D362" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E362" t="s">
         <v>440</v>
@@ -14247,7 +14253,7 @@
         <v>437</v>
       </c>
       <c r="G362" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="H362" s="9" t="s">
         <v>438</v>
@@ -14262,13 +14268,13 @@
         <v>338</v>
       </c>
       <c r="B363" s="18" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C363" s="11" t="s">
         <v>364</v>
       </c>
       <c r="D363" s="18" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E363" t="s">
         <v>189</v>
@@ -14277,7 +14283,7 @@
         <v>189</v>
       </c>
       <c r="G363" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="H363" s="9" t="s">
         <v>438</v>

</xml_diff>